<commit_message>
* Fixed how the ExcelReadUtils handle formula values * Added new class ExcelFormulaEvaluator for easy formula evaluation
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test1.xlsx
+++ b/src/test/resources/excel/test1.xlsx
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -396,6 +396,30 @@
     <row r="4" spans="1:4">
       <c r="D4" s="3">
         <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="str">
+        <f>"abc"</f>
+        <v>abc</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6">
+        <f>4711</f>
+        <v>4711</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="D8" t="b">
+        <f>C7</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>